<commit_message>
feat: add missing error check
</commit_message>
<xml_diff>
--- a/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
+++ b/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -482,10 +482,30 @@
         <v>6</v>
       </c>
       <c r="E8" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="F8" s="1">
         <v>15.0</v>
       </c>
-      <c r="F8" s="1">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
         <v>16.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: restart clean branch
</commit_message>
<xml_diff>
--- a/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
+++ b/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -482,10 +482,30 @@
         <v>6</v>
       </c>
       <c r="E8" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="F8" s="1">
         <v>15.0</v>
       </c>
-      <c r="F8" s="1">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
         <v>16.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: restart clean branch (#847)
</commit_message>
<xml_diff>
--- a/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
+++ b/packages/server/__tests__/db/testAgencyUploadErrors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -482,10 +482,30 @@
         <v>6</v>
       </c>
       <c r="E8" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="F8" s="1">
         <v>15.0</v>
       </c>
-      <c r="F8" s="1">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
         <v>16.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>